<commit_message>
Added UI of project
</commit_message>
<xml_diff>
--- a/Code/results_extra.xlsx
+++ b/Code/results_extra.xlsx
@@ -13,7 +13,199 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="192">
+  <si>
+    <t>final_1</t>
+  </si>
+  <si>
+    <t>final_2</t>
+  </si>
+  <si>
+    <t>final_3</t>
+  </si>
+  <si>
+    <t>final_4</t>
+  </si>
+  <si>
+    <t>final_5</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Contrast</t>
+  </si>
+  <si>
+    <t>Correlation</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Homogeneity</t>
+  </si>
+  <si>
+    <t>Actual Condition</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
   <si>
     <t>final_1</t>
   </si>
@@ -417,7 +609,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -429,16 +621,20 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,19 +656,19 @@
   <sheetData>
     <row r="3">
       <c r="B3" s="0" t="s">
-        <v>96</v>
+        <v>160</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>97</v>
+        <v>161</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>98</v>
+        <v>162</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>99</v>
+        <v>163</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>100</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4">
@@ -489,7 +685,7 @@
         <v>0.99783474705430986</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>101</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5">
@@ -506,7 +702,7 @@
         <v>0.99820884084435313</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>101</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6">
@@ -523,7 +719,7 @@
         <v>0.99647166968139433</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>102</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7">
@@ -540,7 +736,7 @@
         <v>0.99614439733633753</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>102</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8">
@@ -557,7 +753,7 @@
         <v>0.99968658298050017</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>103</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9">
@@ -574,7 +770,7 @@
         <v>0.99708751501391757</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>104</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10">
@@ -591,7 +787,7 @@
         <v>0.99460550065980002</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>104</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11">
@@ -608,7 +804,7 @@
         <v>0.99355679584607792</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>104</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12">
@@ -625,7 +821,7 @@
         <v>0.99426102860025845</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>104</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13">
@@ -642,7 +838,7 @@
         <v>0.99773441538648222</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>105</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14">
@@ -659,7 +855,7 @@
         <v>0.99758630673397475</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>106</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15">
@@ -676,7 +872,7 @@
         <v>0.99464897771585892</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>107</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16">
@@ -693,7 +889,7 @@
         <v>0.99704069356893121</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>107</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17">
@@ -710,7 +906,7 @@
         <v>0.99787105756266681</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18">
@@ -727,7 +923,7 @@
         <v>0.99610808682798102</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>109</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19">
@@ -744,7 +940,7 @@
         <v>0.99709229271238553</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>110</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20">
@@ -761,7 +957,7 @@
         <v>0.99815628616120533</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>111</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21">
@@ -778,7 +974,7 @@
         <v>0.99865555565110964</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>112</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22">
@@ -795,7 +991,7 @@
         <v>0.99537662119253267</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>113</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23">
@@ -812,7 +1008,7 @@
         <v>0.99253006844530833</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>114</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24">
@@ -829,7 +1025,7 @@
         <v>0.99654429069810779</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>115</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25">
@@ -846,7 +1042,7 @@
         <v>0.99729677820681495</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>116</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26">
@@ -863,7 +1059,7 @@
         <v>0.99773441538648222</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>117</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27">
@@ -880,7 +1076,7 @@
         <v>0.99827859524198559</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>118</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28">
@@ -897,7 +1093,7 @@
         <v>0.99898665015494081</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>119</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29">
@@ -912,7 +1108,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>120</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30">
@@ -927,7 +1123,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>120</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31">
@@ -944,7 +1140,7 @@
         <v>0.99556342920263086</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>120</v>
+        <v>184</v>
       </c>
     </row>
     <row r="32">
@@ -961,7 +1157,7 @@
         <v>0.99629059490945782</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>121</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33">
@@ -978,7 +1174,7 @@
         <v>0.99681040850277436</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>122</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34">
@@ -995,7 +1191,7 @@
         <v>0.99625906209956927</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>123</v>
+        <v>187</v>
       </c>
     </row>
     <row r="35">
@@ -1012,7 +1208,7 @@
         <v>0.99804878794567564</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>124</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36">
@@ -1029,7 +1225,7 @@
         <v>0.99807602082694302</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>124</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37">
@@ -1046,7 +1242,7 @@
         <v>0.99863883370647155</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>124</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38">
@@ -1063,7 +1259,7 @@
         <v>0.99861637852367202</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>124</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39">
@@ -1080,7 +1276,7 @@
         <v>0.99802537722318241</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>124</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40">
@@ -1097,7 +1293,7 @@
         <v>0.99889348503481523</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>124</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41">
@@ -1114,7 +1310,7 @@
         <v>0.99801343297701262</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>124</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42">
@@ -1131,7 +1327,7 @@
         <v>0.99853420211002275</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>124</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43">
@@ -1148,7 +1344,7 @@
         <v>0.99778601452993654</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>124</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44">
@@ -1165,7 +1361,7 @@
         <v>0.99515636929315865</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>125</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45">
@@ -1182,7 +1378,7 @@
         <v>0.9968467190111312</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>125</v>
+        <v>189</v>
       </c>
     </row>
     <row r="46">
@@ -1199,7 +1395,7 @@
         <v>0.99905067131441172</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>125</v>
+        <v>189</v>
       </c>
     </row>
     <row r="47">
@@ -1216,7 +1412,7 @@
         <v>0.99661500063543385</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>126</v>
+        <v>190</v>
       </c>
     </row>
     <row r="48">
@@ -1233,7 +1429,7 @@
         <v>0.99673109870820586</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>127</v>
+        <v>191</v>
       </c>
     </row>
     <row r="49">
@@ -1250,7 +1446,7 @@
         <v>0.99603833243034834</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>127</v>
+        <v>191</v>
       </c>
     </row>
     <row r="50">
@@ -1267,7 +1463,7 @@
         <v>0.99682091943940399</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>127</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51">
@@ -1284,7 +1480,7 @@
         <v>0.9966498778342503</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>127</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52">
@@ -1301,7 +1497,7 @@
         <v>0.99753375205082695</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>127</v>
+        <v>191</v>
       </c>
     </row>
     <row r="53">
@@ -1318,7 +1514,7 @@
         <v>0.9949518837987289</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>127</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
produce csv file for svm using Hammouche
</commit_message>
<xml_diff>
--- a/Code/results_extra.xlsx
+++ b/Code/results_extra.xlsx
@@ -13,7 +13,199 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="256">
+  <si>
+    <t>final_1</t>
+  </si>
+  <si>
+    <t>final_2</t>
+  </si>
+  <si>
+    <t>final_3</t>
+  </si>
+  <si>
+    <t>final_4</t>
+  </si>
+  <si>
+    <t>final_5</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Contrast</t>
+  </si>
+  <si>
+    <t>Correlation</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Homogeneity</t>
+  </si>
+  <si>
+    <t>Actual Condition</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
   <si>
     <t>final_1</t>
   </si>
@@ -609,7 +801,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -623,11 +815,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -635,6 +829,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,25 +846,25 @@
     <col min="2" max="2" width="14.7109375" customWidth="true"/>
     <col min="3" max="3" width="12.7109375" customWidth="true"/>
     <col min="4" max="4" width="12.7109375" customWidth="true"/>
-    <col min="5" max="5" width="12.7109375" customWidth="true"/>
-    <col min="6" max="6" width="14.89453125" customWidth="true"/>
+    <col min="5" max="5" width="13.140625" customWidth="true"/>
+    <col min="6" max="6" width="15.85546875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="3">
       <c r="B3" s="0" t="s">
-        <v>160</v>
+        <v>224</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>161</v>
+        <v>225</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>162</v>
+        <v>226</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>163</v>
+        <v>227</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>164</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4">
@@ -685,7 +881,7 @@
         <v>0.99783474705430986</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>165</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5">
@@ -702,7 +898,7 @@
         <v>0.99820884084435313</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>165</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6">
@@ -719,7 +915,7 @@
         <v>0.99647166968139433</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>166</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7">
@@ -736,7 +932,7 @@
         <v>0.99614439733633753</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>166</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8">
@@ -753,7 +949,7 @@
         <v>0.99968658298050017</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>167</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9">
@@ -770,7 +966,7 @@
         <v>0.99708751501391757</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>168</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10">
@@ -787,7 +983,7 @@
         <v>0.99460550065980002</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>168</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11">
@@ -804,7 +1000,7 @@
         <v>0.99355679584607792</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>168</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12">
@@ -821,7 +1017,7 @@
         <v>0.99426102860025845</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>168</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13">
@@ -838,7 +1034,7 @@
         <v>0.99773441538648222</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>169</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14">
@@ -855,7 +1051,7 @@
         <v>0.99758630673397475</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>170</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15">
@@ -872,7 +1068,7 @@
         <v>0.99464897771585892</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>171</v>
+        <v>235</v>
       </c>
     </row>
     <row r="16">
@@ -889,7 +1085,7 @@
         <v>0.99704069356893121</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>171</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17">
@@ -906,7 +1102,7 @@
         <v>0.99787105756266681</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>172</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18">
@@ -923,7 +1119,7 @@
         <v>0.99610808682798102</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>173</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19">
@@ -940,7 +1136,7 @@
         <v>0.99709229271238553</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>174</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20">
@@ -957,7 +1153,7 @@
         <v>0.99815628616120533</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>175</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21">
@@ -974,7 +1170,7 @@
         <v>0.99865555565110964</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>176</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22">
@@ -991,7 +1187,7 @@
         <v>0.99537662119253267</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23">
@@ -1008,7 +1204,7 @@
         <v>0.99253006844530833</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>178</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24">
@@ -1025,7 +1221,7 @@
         <v>0.99654429069810779</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>179</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25">
@@ -1042,7 +1238,7 @@
         <v>0.99729677820681495</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>180</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26">
@@ -1059,7 +1255,7 @@
         <v>0.99773441538648222</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>181</v>
+        <v>245</v>
       </c>
     </row>
     <row r="27">
@@ -1076,7 +1272,7 @@
         <v>0.99827859524198559</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>182</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28">
@@ -1093,7 +1289,7 @@
         <v>0.99898665015494081</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>183</v>
+        <v>247</v>
       </c>
     </row>
     <row r="29">
@@ -1108,7 +1304,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>184</v>
+        <v>248</v>
       </c>
     </row>
     <row r="30">
@@ -1123,7 +1319,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>184</v>
+        <v>248</v>
       </c>
     </row>
     <row r="31">
@@ -1140,7 +1336,7 @@
         <v>0.99556342920263086</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>184</v>
+        <v>248</v>
       </c>
     </row>
     <row r="32">
@@ -1157,7 +1353,7 @@
         <v>0.99629059490945782</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>185</v>
+        <v>249</v>
       </c>
     </row>
     <row r="33">
@@ -1174,7 +1370,7 @@
         <v>0.99681040850277436</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>186</v>
+        <v>250</v>
       </c>
     </row>
     <row r="34">
@@ -1191,7 +1387,7 @@
         <v>0.99625906209956927</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>187</v>
+        <v>251</v>
       </c>
     </row>
     <row r="35">
@@ -1208,7 +1404,7 @@
         <v>0.99804878794567564</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>188</v>
+        <v>252</v>
       </c>
     </row>
     <row r="36">
@@ -1225,7 +1421,7 @@
         <v>0.99807602082694302</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>188</v>
+        <v>252</v>
       </c>
     </row>
     <row r="37">
@@ -1242,7 +1438,7 @@
         <v>0.99863883370647155</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>188</v>
+        <v>252</v>
       </c>
     </row>
     <row r="38">
@@ -1259,7 +1455,7 @@
         <v>0.99861637852367202</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>188</v>
+        <v>252</v>
       </c>
     </row>
     <row r="39">
@@ -1276,7 +1472,7 @@
         <v>0.99802537722318241</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>188</v>
+        <v>252</v>
       </c>
     </row>
     <row r="40">
@@ -1293,7 +1489,7 @@
         <v>0.99889348503481523</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>188</v>
+        <v>252</v>
       </c>
     </row>
     <row r="41">
@@ -1310,7 +1506,7 @@
         <v>0.99801343297701262</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>188</v>
+        <v>252</v>
       </c>
     </row>
     <row r="42">
@@ -1327,7 +1523,7 @@
         <v>0.99853420211002275</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>188</v>
+        <v>252</v>
       </c>
     </row>
     <row r="43">
@@ -1344,7 +1540,7 @@
         <v>0.99778601452993654</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>188</v>
+        <v>252</v>
       </c>
     </row>
     <row r="44">
@@ -1361,7 +1557,7 @@
         <v>0.99515636929315865</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>189</v>
+        <v>253</v>
       </c>
     </row>
     <row r="45">
@@ -1378,7 +1574,7 @@
         <v>0.9968467190111312</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>189</v>
+        <v>253</v>
       </c>
     </row>
     <row r="46">
@@ -1395,7 +1591,7 @@
         <v>0.99905067131441172</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>189</v>
+        <v>253</v>
       </c>
     </row>
     <row r="47">
@@ -1412,7 +1608,7 @@
         <v>0.99661500063543385</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>190</v>
+        <v>254</v>
       </c>
     </row>
     <row r="48">
@@ -1429,7 +1625,7 @@
         <v>0.99673109870820586</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>191</v>
+        <v>255</v>
       </c>
     </row>
     <row r="49">
@@ -1446,7 +1642,7 @@
         <v>0.99603833243034834</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>191</v>
+        <v>255</v>
       </c>
     </row>
     <row r="50">
@@ -1463,7 +1659,7 @@
         <v>0.99682091943940399</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>191</v>
+        <v>255</v>
       </c>
     </row>
     <row r="51">
@@ -1480,7 +1676,7 @@
         <v>0.9966498778342503</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>191</v>
+        <v>255</v>
       </c>
     </row>
     <row r="52">
@@ -1497,7 +1693,7 @@
         <v>0.99753375205082695</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>191</v>
+        <v>255</v>
       </c>
     </row>
     <row r="53">
@@ -1514,7 +1710,7 @@
         <v>0.9949518837987289</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>191</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>